<commit_message>
Update simulation logic to include exposure time calculations and enhance output file naming with timestamps; refactor emission factor calculations and adjust polymer density values.
</commit_message>
<xml_diff>
--- a/Gewässersteckbriefe mit kSt.xlsx
+++ b/Gewässersteckbriefe mit kSt.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Nachwuchsforscher\Lucas Kurzweg\Promotion\Abrasion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arulu410\Desktop\Microplastic-River-Abrasion-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8250"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7670"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="92">
   <si>
     <t>Typ und Bezeichnung</t>
   </si>
@@ -279,6 +279,27 @@
   </si>
   <si>
     <t>k_St (max)</t>
+  </si>
+  <si>
+    <t>0.3</t>
+  </si>
+  <si>
+    <t>0.8</t>
+  </si>
+  <si>
+    <t>0.45</t>
+  </si>
+  <si>
+    <t>0.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.8</t>
+  </si>
+  <si>
+    <t>Water level in m</t>
   </si>
 </sst>
 </file>
@@ -348,7 +369,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -366,6 +387,12 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -648,10 +675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -661,13 +688,14 @@
     <col min="3" max="3" width="17.1796875" style="6" customWidth="1"/>
     <col min="4" max="4" width="13.54296875" style="1" customWidth="1"/>
     <col min="5" max="5" width="14" style="1" customWidth="1"/>
-    <col min="6" max="6" width="43.90625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="21.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="125.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="10.90625" style="1"/>
+    <col min="6" max="6" width="16.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="43.90625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="21.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="125.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="10.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -684,16 +712,19 @@
         <v>84</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -709,17 +740,20 @@
       <c r="E2" s="3">
         <v>40</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="3">
+        <v>0</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:9" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -735,17 +769,20 @@
       <c r="E3" s="3">
         <v>50</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="3">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:9" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -761,17 +798,20 @@
       <c r="E4" s="3">
         <v>30</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="3">
+        <v>0</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:9" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
@@ -787,17 +827,20 @@
       <c r="E5" s="3">
         <v>35</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="3">
+        <v>0</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="H5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="I5" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:9" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
@@ -814,16 +857,19 @@
         <v>30</v>
       </c>
       <c r="F6" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="H6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="I6" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:9" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="3" t="s">
         <v>20</v>
       </c>
@@ -840,16 +886,19 @@
         <v>50</v>
       </c>
       <c r="F7" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="H7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="I7" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:9" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="3" t="s">
         <v>23</v>
       </c>
@@ -866,16 +915,19 @@
         <v>60</v>
       </c>
       <c r="F8" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="H8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="I8" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:9" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="3" t="s">
         <v>26</v>
       </c>
@@ -892,16 +944,19 @@
         <v>50</v>
       </c>
       <c r="F9" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="H9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="I9" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:9" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="3" t="s">
         <v>29</v>
       </c>
@@ -918,16 +973,19 @@
         <v>50</v>
       </c>
       <c r="F10" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="H10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="I10" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:9" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="3" t="s">
         <v>32</v>
       </c>
@@ -944,16 +1002,19 @@
         <v>40</v>
       </c>
       <c r="F11" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="H11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="I11" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:9" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="3" t="s">
         <v>35</v>
       </c>
@@ -970,16 +1031,19 @@
         <v>35</v>
       </c>
       <c r="F12" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="H12" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="I12" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:9" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="3" t="s">
         <v>38</v>
       </c>
@@ -995,17 +1059,20 @@
       <c r="E13" s="3">
         <v>35</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="H13" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="I13" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:9" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="3" t="s">
         <v>41</v>
       </c>
@@ -1022,16 +1089,19 @@
         <v>50</v>
       </c>
       <c r="F14" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G14" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="H14" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="I14" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:9" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="3" t="s">
         <v>45</v>
       </c>
@@ -1048,16 +1118,19 @@
         <v>50</v>
       </c>
       <c r="F15" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="H15" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="I15" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:9" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="3" t="s">
         <v>48</v>
       </c>
@@ -1073,17 +1146,20 @@
       <c r="E16" s="3">
         <v>50</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="G16" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="H16" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="I16" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:9" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="3" t="s">
         <v>49</v>
       </c>
@@ -1100,16 +1176,19 @@
         <v>35</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>50</v>
+        <v>85</v>
       </c>
       <c r="G17" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H17" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="I17" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:9" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="3" t="s">
         <v>52</v>
       </c>
@@ -1126,16 +1205,19 @@
         <v>35</v>
       </c>
       <c r="F18" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G18" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="H18" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="H18" s="3" t="s">
+      <c r="I18" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:9" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="3" t="s">
         <v>55</v>
       </c>
@@ -1152,16 +1234,19 @@
         <v>60</v>
       </c>
       <c r="F19" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G19" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="H19" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="H19" s="3" t="s">
+      <c r="I19" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:9" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="3" t="s">
         <v>58</v>
       </c>
@@ -1177,17 +1262,20 @@
       <c r="E20" s="3">
         <v>45</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="G20" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="H20" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="I20" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:9" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="3" t="s">
         <v>60</v>
       </c>
@@ -1203,17 +1291,20 @@
       <c r="E21" s="3">
         <v>60</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" s="3">
+        <v>0</v>
+      </c>
+      <c r="G21" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="H21" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="H21" s="3" t="s">
+      <c r="I21" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:9" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="3" t="s">
         <v>63</v>
       </c>
@@ -1229,17 +1320,20 @@
       <c r="E22" s="3">
         <v>50</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F22" s="3">
+        <v>0</v>
+      </c>
+      <c r="G22" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="G22" s="3" t="s">
+      <c r="H22" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="H22" s="3" t="s">
+      <c r="I22" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:9" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="3" t="s">
         <v>65</v>
       </c>
@@ -1256,16 +1350,19 @@
         <v>50</v>
       </c>
       <c r="F23" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G23" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="G23" s="3" t="s">
+      <c r="H23" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="H23" s="3" t="s">
+      <c r="I23" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:9" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="3" t="s">
         <v>69</v>
       </c>
@@ -1281,17 +1378,20 @@
       <c r="E24" s="3">
         <v>50</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F24" s="3">
+        <v>0</v>
+      </c>
+      <c r="G24" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="G24" s="3" t="s">
+      <c r="H24" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="H24" s="3" t="s">
+      <c r="I24" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:9" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="3" t="s">
         <v>71</v>
       </c>
@@ -1308,16 +1408,19 @@
         <v>50</v>
       </c>
       <c r="F25" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G25" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="H25" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="H25" s="3" t="s">
+      <c r="I25" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:9" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="3" t="s">
         <v>73</v>
       </c>
@@ -1333,13 +1436,16 @@
       <c r="E26" s="3">
         <v>50</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="F26" s="3">
+        <v>0</v>
+      </c>
+      <c r="G26" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="G26" s="3" t="s">
+      <c r="H26" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="H26" s="3" t="s">
+      <c r="I26" s="3" t="s">
         <v>75</v>
       </c>
     </row>

</xml_diff>